<commit_message>
inclui regioes na tabela de ufs
</commit_message>
<xml_diff>
--- a/dados/tab_ufs.xlsx
+++ b/dados/tab_ufs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tiago.pereira\Documents\GitHub\fluxo-rec-desp\dados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tiago.pereira\Documents\GitHub\estatais-estados\dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FBBE493-2FD4-40B2-A929-B62FED72E2A7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7753F2B6-F3B5-4864-9B38-1ADC43AF5BB7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23880" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{06E5B434-546D-441A-8AD3-4681C62FB42B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{06E5B434-546D-441A-8AD3-4681C62FB42B}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="36">
   <si>
     <t>UF</t>
   </si>
@@ -118,6 +118,27 @@
   </si>
   <si>
     <t>CODUF</t>
+  </si>
+  <si>
+    <t>REGIAO</t>
+  </si>
+  <si>
+    <t>CODREG</t>
+  </si>
+  <si>
+    <t>Norte</t>
+  </si>
+  <si>
+    <t>Nordeste</t>
+  </si>
+  <si>
+    <t>Sudeste</t>
+  </si>
+  <si>
+    <t>Sul</t>
+  </si>
+  <si>
+    <t>Centro-oeste</t>
   </si>
 </sst>
 </file>
@@ -469,240 +490,407 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{831FC411-1B9D-4464-BA26-4414F7B8ECF3}">
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>28</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>11</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>12</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>13</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>14</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>15</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>16</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>17</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>21</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>22</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>23</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>24</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>25</v>
       </c>
       <c r="B13" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>26</v>
       </c>
       <c r="B14" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>27</v>
       </c>
       <c r="B15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>28</v>
       </c>
       <c r="B16" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>29</v>
       </c>
       <c r="B17" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>31</v>
       </c>
       <c r="B18" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>32</v>
       </c>
       <c r="B19" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>33</v>
       </c>
       <c r="B20" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>35</v>
       </c>
       <c r="B21" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>41</v>
       </c>
       <c r="B22" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>42</v>
       </c>
       <c r="B23" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>43</v>
       </c>
       <c r="B24" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>50</v>
       </c>
       <c r="B25" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>51</v>
       </c>
       <c r="B26" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>35</v>
+      </c>
+      <c r="D26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>52</v>
       </c>
       <c r="B27" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>35</v>
+      </c>
+      <c r="D27">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>53</v>
       </c>
       <c r="B28" t="s">
         <v>27</v>
+      </c>
+      <c r="C28" t="s">
+        <v>35</v>
+      </c>
+      <c r="D28">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>